<commit_message>
Add coments and make better corner detection
</commit_message>
<xml_diff>
--- a/test/dom_clr/meta_data.xlsx
+++ b/test/dom_clr/meta_data.xlsx
@@ -540,82 +540,82 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>73.62410059253746</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>181.1961237301674</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>146.3996190745278</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>219.2887185022159</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>200.6213942755026</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>125.159675438266</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>86.60063897763453</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>38.43218849842226</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>123.4248003194851</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>44.23406337940434</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>61.99730820996579</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>166.1550226355252</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>38.2699642431316</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>14.64673553173402</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>93.61826248178487</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.05692088156017124</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.1091908461497807</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.08498493737117488</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.1060197663971249</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.05422546377041383</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0.1063897257016014</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>0.02029491041699698</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>0.01733523598118493</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>642</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -623,13 +623,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>73.62545858613032</v>
+        <v>73.62410059253746</v>
       </c>
       <c r="C3">
-        <v>181.2015486100503</v>
+        <v>181.1961237301674</v>
       </c>
       <c r="D3">
-        <v>146.4034323409416</v>
+        <v>146.3996190745278</v>
       </c>
       <c r="E3">
         <v>219.2887185022159</v>
@@ -641,13 +641,13 @@
         <v>125.159675438266</v>
       </c>
       <c r="H3">
-        <v>86.60724701370178</v>
+        <v>86.60545657905126</v>
       </c>
       <c r="I3">
-        <v>38.43793695819156</v>
+        <v>38.43600703045831</v>
       </c>
       <c r="J3">
-        <v>123.4323438935683</v>
+        <v>123.4291763202008</v>
       </c>
       <c r="K3">
         <v>44.23617229562796</v>
@@ -659,13 +659,13 @@
         <v>166.1586514929206</v>
       </c>
       <c r="N3">
-        <v>38.28630979949535</v>
+        <v>38.27906822842785</v>
       </c>
       <c r="O3">
-        <v>14.65341097070386</v>
+        <v>14.65614453049086</v>
       </c>
       <c r="P3">
-        <v>93.6291934096417</v>
+        <v>93.62921050889517</v>
       </c>
       <c r="Q3">
         <v>0.05692088156017124</v>
@@ -706,49 +706,49 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>111.5412676077615</v>
+        <v>109.6901181963495</v>
       </c>
       <c r="C4">
-        <v>101.1812446098662</v>
+        <v>97.67287850589261</v>
       </c>
       <c r="D4">
-        <v>190.3341957544783</v>
+        <v>186.4254334410942</v>
       </c>
       <c r="E4">
-        <v>108.0535913477953</v>
+        <v>87.42396519736401</v>
       </c>
       <c r="F4">
-        <v>95.65771052588909</v>
+        <v>104.9072995969533</v>
       </c>
       <c r="G4">
-        <v>183.0366328790684</v>
+        <v>154.5306762203259</v>
       </c>
       <c r="H4">
-        <v>87.19845225603338</v>
+        <v>33.1519060454403</v>
       </c>
       <c r="I4">
-        <v>105.3266002098621</v>
+        <v>43.12033115132662</v>
       </c>
       <c r="J4">
-        <v>154.2056663168886</v>
+        <v>82.43357720447598</v>
       </c>
       <c r="K4">
-        <v>33.15479399307218</v>
+        <v>74.51240661686211</v>
       </c>
       <c r="L4">
-        <v>43.12360415864276</v>
+        <v>81.89701173959355</v>
       </c>
       <c r="M4">
-        <v>82.44060454371356</v>
+        <v>127.7704108858022</v>
       </c>
       <c r="N4">
-        <v>74.54107309279702</v>
+        <v>50.21404158360141</v>
       </c>
       <c r="O4">
-        <v>81.85820796165532</v>
+        <v>59.29592708629858</v>
       </c>
       <c r="P4">
-        <v>127.8506190919949</v>
+        <v>109.0707775562541</v>
       </c>
       <c r="Q4">
         <v>0.0003171079752655779</v>

</xml_diff>